<commit_message>
users.json merged to contact.xlsx
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20417"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanda\Desktop\broadcast-panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C9349-B0BA-480A-9C6D-3BCB16CCCFFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB35543B-945C-4976-8A19-40F703E8DAA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+  <si>
+    <t>WhatsApp JID</t>
+  </si>
   <si>
     <t>Contractors</t>
   </si>
@@ -30,31 +33,29 @@
   <si>
     <t>Retailers</t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,14 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -81,38 +75,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -135,28 +111,28 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -258,6 +234,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -268,31 +245,27 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -314,7 +287,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -372,7 +345,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -385,12 +358,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -402,123 +376,119 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.75" customWidth="1"/>
+    <col min="2" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>917021217553</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>917021217553</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>917021217553</v>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:D1 A5:D5 B3 D3 A4:B4 D4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>